<commit_message>
Finished GIS regions and upload
</commit_message>
<xml_diff>
--- a/Bunderbuurten veghel model/_mvlv_transformers.xlsx
+++ b/Bunderbuurten veghel model/_mvlv_transformers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Buurtmodel-Bunderbuurten-Veghel\Bunderbuurten veghel model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78544352-974A-4E0F-B49C-6DF9FB318FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CDD1BA-566C-49B5-934F-1CE187B8A59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22140" yWindow="1560" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="552" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mvlv_transformers" sheetId="1" r:id="rId1"/>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -623,10 +623,10 @@
         <v>10</v>
       </c>
       <c r="P1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" t="s">
         <v>55</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -677,10 +677,10 @@
         <v>11</v>
       </c>
       <c r="P2">
-        <v>51.621000000000002</v>
+        <v>5.5643530008095192</v>
       </c>
       <c r="Q2">
-        <v>5.5640000000000001</v>
+        <v>51.621006743843317</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -731,10 +731,10 @@
         <v>11</v>
       </c>
       <c r="P3">
-        <v>51.624000000000002</v>
+        <v>5.5530209761477183</v>
       </c>
       <c r="Q3">
-        <v>5.5529999999999999</v>
+        <v>51.624337024457091</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -785,10 +785,10 @@
         <v>11</v>
       </c>
       <c r="P4">
-        <v>51.621000000000002</v>
+        <v>5.5504170565747302</v>
       </c>
       <c r="Q4">
-        <v>5.55</v>
+        <v>51.62112197421213</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -839,10 +839,10 @@
         <v>11</v>
       </c>
       <c r="P5">
-        <v>51.624000000000002</v>
+        <v>5.5494637429464388</v>
       </c>
       <c r="Q5">
-        <v>5.5490000000000004</v>
+        <v>51.623510017791183</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -893,10 +893,10 @@
         <v>11</v>
       </c>
       <c r="P6">
-        <v>51.622</v>
+        <v>5.5516757109692731</v>
       </c>
       <c r="Q6">
-        <v>5.5519999999999996</v>
+        <v>51.622488359419222</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -947,10 +947,10 @@
         <v>11</v>
       </c>
       <c r="P7">
-        <v>51.621000000000002</v>
+        <v>5.5621971334594589</v>
       </c>
       <c r="Q7">
-        <v>5.5620000000000003</v>
+        <v>51.621278156696327</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -1001,10 +1001,10 @@
         <v>11</v>
       </c>
       <c r="P8">
-        <v>51.624000000000002</v>
+        <v>5.5556037890367023</v>
       </c>
       <c r="Q8">
-        <v>5.556</v>
+        <v>51.624107718459797</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -1055,10 +1055,10 @@
         <v>11</v>
       </c>
       <c r="P9">
-        <v>51.627000000000002</v>
+        <v>5.5492819656122689</v>
       </c>
       <c r="Q9">
-        <v>5.5490000000000004</v>
+        <v>51.626746665451911</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -1109,10 +1109,10 @@
         <v>11</v>
       </c>
       <c r="P10">
-        <v>51.618000000000002</v>
+        <v>5.5586866183863224</v>
       </c>
       <c r="Q10">
-        <v>5.5590000000000002</v>
+        <v>51.618183633872547</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -1163,10 +1163,10 @@
         <v>11</v>
       </c>
       <c r="P11">
-        <v>51.628</v>
+        <v>5.5566792520004826</v>
       </c>
       <c r="Q11">
-        <v>5.5570000000000004</v>
+        <v>51.627937000342328</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -1217,10 +1217,10 @@
         <v>11</v>
       </c>
       <c r="P12">
-        <v>51.625999999999998</v>
+        <v>5.5482485553741601</v>
       </c>
       <c r="Q12">
-        <v>5.548</v>
+        <v>51.626404317432439</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -1271,10 +1271,10 @@
         <v>11</v>
       </c>
       <c r="P13">
-        <v>51.627000000000002</v>
+        <v>5.5530852770255033</v>
       </c>
       <c r="Q13">
-        <v>5.5529999999999999</v>
+        <v>51.626830630646523</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -1325,10 +1325,10 @@
         <v>11</v>
       </c>
       <c r="P14">
-        <v>51.62</v>
+        <v>5.5548837969885767</v>
       </c>
       <c r="Q14">
-        <v>5.5549999999999997</v>
+        <v>51.619672958373222</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -1379,10 +1379,10 @@
         <v>11</v>
       </c>
       <c r="P15">
-        <v>51.621000000000002</v>
+        <v>5.5534403477137237</v>
       </c>
       <c r="Q15">
-        <v>5.5529999999999999</v>
+        <v>51.621052806352218</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -1433,10 +1433,10 @@
         <v>11</v>
       </c>
       <c r="P16">
-        <v>51.622999999999998</v>
+        <v>5.5620234232032573</v>
       </c>
       <c r="Q16">
-        <v>5.5620000000000003</v>
+        <v>51.623321770056393</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -1487,10 +1487,10 @@
         <v>11</v>
       </c>
       <c r="P17">
-        <v>51.622</v>
+        <v>5.5572400179952099</v>
       </c>
       <c r="Q17">
-        <v>5.5570000000000004</v>
+        <v>51.621776591367023</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
@@ -1541,10 +1541,10 @@
         <v>11</v>
       </c>
       <c r="P18">
-        <v>51.62</v>
+        <v>5.5607552792176378</v>
       </c>
       <c r="Q18">
-        <v>5.5609999999999999</v>
+        <v>51.619868274254138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>